<commit_message>
update files for underpressure paper
</commit_message>
<xml_diff>
--- a/underpressure/Table_of_Satellites.xlsx
+++ b/underpressure/Table_of_Satellites.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/Desktop/icymoons_thermal_stress/underpressure/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1063FF6C-1496-F542-982F-78EB56B46F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A2FB804-ADDD-D747-AFEC-A50AA8656E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3480" yWindow="2620" windowWidth="27640" windowHeight="16940" xr2:uid="{F8F1A65A-EB63-5142-8E37-A60CFA520D03}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <r>
       <t>D</t>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>Rc, km</t>
+  </si>
+  <si>
+    <t>Triton</t>
   </si>
 </sst>
 </file>
@@ -524,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF91998E-C3D0-274F-B194-D271C8BDB944}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -952,6 +955,20 @@
         <v>1.46</v>
       </c>
     </row>
+    <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="4">
+        <v>1028</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0.76</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0.75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>